<commit_message>
ZFIN-6747 update workbook for zebra share
</commit_message>
<xml_diff>
--- a/home/zf_info/zebraShareSubmission.xlsx
+++ b/home/zf_info/zebraShareSubmission.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoregon-my.sharepoint.com/personal/leyla_uoregon_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/administrator/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{EFC879CE-2E08-D246-9987-13560E3C43D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{05686A92-7E13-B747-B6AC-598FF48802B3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{52A33CEA-2ADA-C74F-BC46-F0DC48A09E9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14180" yWindow="460" windowWidth="25320" windowHeight="19660" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4400" yWindow="460" windowWidth="31720" windowHeight="17340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -2848,9 +2848,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2875,8 +2872,55 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2886,12 +2930,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2910,19 +2948,10 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2943,38 +2972,9 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2993,10 +2993,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3277,7 +3273,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="16" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:26" ht="32" x14ac:dyDescent="0.35">
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="121" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3317,22 +3313,22 @@
       <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:26" ht="25" x14ac:dyDescent="0.3">
-      <c r="B12" s="116" t="s">
+      <c r="B12" s="115" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="121" t="s">
+      <c r="B13" s="120" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="19" x14ac:dyDescent="0.25">
-      <c r="B14" s="120" t="s">
+      <c r="B14" s="119" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="119"/>
+      <c r="B15" s="118"/>
     </row>
     <row r="16" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
@@ -3378,7 +3374,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="60" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B20" s="118" t="s">
+      <c r="B20" s="117" t="s">
         <v>219</v>
       </c>
     </row>
@@ -3396,7 +3392,7 @@
       <c r="A22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="20" x14ac:dyDescent="0.25">
-      <c r="B23" s="117" t="s">
+      <c r="B23" s="116" t="s">
         <v>170</v>
       </c>
     </row>
@@ -4397,9 +4393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:MZ1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4451,14 +4445,14 @@
       <c r="I1" s="73"/>
       <c r="J1" s="75"/>
       <c r="K1" s="75"/>
-      <c r="L1" s="129" t="s">
+      <c r="L1" s="125" t="s">
         <v>178</v>
       </c>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
-      <c r="O1" s="130"/>
-      <c r="P1" s="130"/>
-      <c r="Q1" s="130"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="126"/>
+      <c r="O1" s="126"/>
+      <c r="P1" s="126"/>
+      <c r="Q1" s="126"/>
       <c r="U1" s="77"/>
       <c r="AL1" s="78"/>
       <c r="AM1" s="78"/>
@@ -4849,14 +4843,14 @@
       <c r="U4" s="77"/>
     </row>
     <row r="5" spans="1:364" s="84" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="129" t="s">
+      <c r="A5" s="125" t="s">
         <v>223</v>
       </c>
-      <c r="B5" s="130"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
       <c r="G5" s="83"/>
       <c r="H5" s="86"/>
       <c r="J5" s="86"/>
@@ -5203,11 +5197,11 @@
       <c r="C6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="125" t="s">
+      <c r="D6" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
       <c r="G6" s="20" t="s">
         <v>7</v>
       </c>
@@ -5283,11 +5277,11 @@
       <c r="AE6" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="AF6" s="127" t="s">
+      <c r="AF6" s="141" t="s">
         <v>126</v>
       </c>
-      <c r="AG6" s="128"/>
-      <c r="AH6" s="128"/>
+      <c r="AG6" s="142"/>
+      <c r="AH6" s="142"/>
       <c r="AI6" s="15" t="s">
         <v>87</v>
       </c>
@@ -5739,7 +5733,7 @@
       <c r="MZ7"/>
     </row>
     <row r="8" spans="1:364" s="19" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="159" t="s">
+      <c r="A8" s="123" t="s">
         <v>225</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -6177,7 +6171,7 @@
       <c r="MZ8"/>
     </row>
     <row r="9" spans="1:364" s="36" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="159" t="s">
+      <c r="A9" s="123" t="s">
         <v>225</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -7937,13 +7931,13 @@
       <c r="MZ12"/>
     </row>
     <row r="13" spans="1:364" s="19" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="133" t="s">
+      <c r="A13" s="145" t="s">
         <v>229</v>
       </c>
-      <c r="B13" s="135" t="s">
+      <c r="B13" s="147" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="135" t="s">
+      <c r="C13" s="147" t="s">
         <v>103</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -7958,16 +7952,16 @@
       <c r="G13" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="131" t="s">
+      <c r="H13" s="143" t="s">
         <v>59</v>
       </c>
       <c r="I13" s="100" t="s">
         <v>157</v>
       </c>
-      <c r="J13" s="135" t="s">
+      <c r="J13" s="147" t="s">
         <v>148</v>
       </c>
-      <c r="K13" s="135">
+      <c r="K13" s="147">
         <v>10</v>
       </c>
       <c r="L13" s="95" t="s">
@@ -7982,70 +7976,70 @@
       <c r="O13" s="97" t="s">
         <v>196</v>
       </c>
-      <c r="P13" s="137" t="s">
+      <c r="P13" s="129" t="s">
         <v>143</v>
       </c>
-      <c r="Q13" s="139" t="s">
+      <c r="Q13" s="149" t="s">
         <v>206</v>
       </c>
-      <c r="R13" s="141" t="s">
+      <c r="R13" s="133" t="s">
         <v>34</v>
       </c>
-      <c r="S13" s="150" t="s">
+      <c r="S13" s="131" t="s">
         <v>129</v>
       </c>
-      <c r="T13" s="141" t="s">
+      <c r="T13" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="U13" s="153" t="s">
+      <c r="U13" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="V13" s="155" t="s">
+      <c r="V13" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="W13" s="115" t="s">
+      <c r="W13" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="X13" s="135" t="s">
+      <c r="X13" s="147" t="s">
         <v>107</v>
       </c>
-      <c r="Y13" s="144" t="s">
+      <c r="Y13" s="153" t="s">
         <v>29</v>
       </c>
-      <c r="Z13" s="141" t="s">
+      <c r="Z13" s="133" t="s">
         <v>30</v>
       </c>
-      <c r="AA13" s="146" t="s">
+      <c r="AA13" s="155" t="s">
         <v>130</v>
       </c>
       <c r="AB13" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="AC13" s="137" t="s">
+      <c r="AC13" s="129" t="s">
         <v>155</v>
       </c>
-      <c r="AD13" s="137" t="s">
+      <c r="AD13" s="129" t="s">
         <v>155</v>
       </c>
-      <c r="AE13" s="137" t="s">
+      <c r="AE13" s="129" t="s">
         <v>155</v>
       </c>
-      <c r="AF13" s="137" t="s">
+      <c r="AF13" s="129" t="s">
         <v>155</v>
       </c>
-      <c r="AG13" s="137" t="s">
+      <c r="AG13" s="129" t="s">
         <v>155</v>
       </c>
-      <c r="AH13" s="137" t="s">
+      <c r="AH13" s="129" t="s">
         <v>155</v>
       </c>
-      <c r="AI13" s="148" t="s">
+      <c r="AI13" s="127" t="s">
         <v>164</v>
       </c>
-      <c r="AJ13" s="148" t="s">
+      <c r="AJ13" s="127" t="s">
         <v>165</v>
       </c>
-      <c r="AK13" s="137" t="s">
+      <c r="AK13" s="129" t="s">
         <v>155</v>
       </c>
       <c r="AL13"/>
@@ -8377,9 +8371,9 @@
       <c r="MZ13"/>
     </row>
     <row r="14" spans="1:364" s="64" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="134"/>
-      <c r="B14" s="136"/>
-      <c r="C14" s="136"/>
+      <c r="A14" s="146"/>
+      <c r="B14" s="148"/>
+      <c r="C14" s="148"/>
       <c r="D14" s="102" t="s">
         <v>40</v>
       </c>
@@ -8392,12 +8386,12 @@
       <c r="G14" s="101" t="s">
         <v>106</v>
       </c>
-      <c r="H14" s="132"/>
+      <c r="H14" s="144"/>
       <c r="I14" s="99" t="s">
         <v>154</v>
       </c>
-      <c r="J14" s="136"/>
-      <c r="K14" s="136"/>
+      <c r="J14" s="148"/>
+      <c r="K14" s="148"/>
       <c r="L14" s="98" t="s">
         <v>199</v>
       </c>
@@ -8410,28 +8404,28 @@
       <c r="O14" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="P14" s="138"/>
-      <c r="Q14" s="140"/>
-      <c r="R14" s="142"/>
-      <c r="S14" s="151"/>
-      <c r="T14" s="152"/>
-      <c r="U14" s="154"/>
-      <c r="V14" s="156"/>
-      <c r="W14" s="114"/>
-      <c r="X14" s="143"/>
-      <c r="Y14" s="145"/>
-      <c r="Z14" s="142"/>
-      <c r="AA14" s="147"/>
+      <c r="P14" s="130"/>
+      <c r="Q14" s="150"/>
+      <c r="R14" s="151"/>
+      <c r="S14" s="132"/>
+      <c r="T14" s="134"/>
+      <c r="U14" s="136"/>
+      <c r="V14" s="138"/>
+      <c r="W14" s="159"/>
+      <c r="X14" s="152"/>
+      <c r="Y14" s="154"/>
+      <c r="Z14" s="151"/>
+      <c r="AA14" s="156"/>
       <c r="AB14" s="108"/>
-      <c r="AC14" s="138"/>
-      <c r="AD14" s="138"/>
-      <c r="AE14" s="138"/>
-      <c r="AF14" s="138"/>
-      <c r="AG14" s="138"/>
-      <c r="AH14" s="138"/>
-      <c r="AI14" s="149"/>
-      <c r="AJ14" s="149"/>
-      <c r="AK14" s="138"/>
+      <c r="AC14" s="130"/>
+      <c r="AD14" s="130"/>
+      <c r="AE14" s="130"/>
+      <c r="AF14" s="130"/>
+      <c r="AG14" s="130"/>
+      <c r="AH14" s="130"/>
+      <c r="AI14" s="128"/>
+      <c r="AJ14" s="128"/>
+      <c r="AK14" s="130"/>
       <c r="AL14" s="55"/>
       <c r="AM14" s="55"/>
       <c r="AN14" s="55"/>
@@ -8775,7 +8769,7 @@
       <c r="K15" s="51"/>
       <c r="L15" s="51"/>
       <c r="M15" s="51"/>
-      <c r="N15" s="123"/>
+      <c r="N15" s="122"/>
       <c r="O15" s="49"/>
       <c r="P15" s="50"/>
       <c r="Q15" s="14"/>
@@ -8817,7 +8811,7 @@
       <c r="K16" s="51"/>
       <c r="L16" s="51"/>
       <c r="M16" s="51"/>
-      <c r="N16" s="123"/>
+      <c r="N16" s="122"/>
       <c r="O16" s="49"/>
       <c r="P16" s="50"/>
       <c r="Q16" s="14"/>
@@ -8826,7 +8820,6 @@
       <c r="T16" s="13"/>
       <c r="U16" s="50"/>
       <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
       <c r="Z16" s="13"/>
@@ -8859,7 +8852,7 @@
       <c r="K17" s="51"/>
       <c r="L17" s="51"/>
       <c r="M17" s="51"/>
-      <c r="N17" s="123"/>
+      <c r="N17" s="122"/>
       <c r="O17" s="49"/>
       <c r="P17" s="50"/>
       <c r="Q17" s="14"/>
@@ -8901,7 +8894,7 @@
       <c r="K18" s="51"/>
       <c r="L18" s="51"/>
       <c r="M18" s="51"/>
-      <c r="N18" s="123"/>
+      <c r="N18" s="122"/>
       <c r="O18" s="49"/>
       <c r="P18" s="50"/>
       <c r="Q18" s="14"/>
@@ -8943,7 +8936,7 @@
       <c r="K19" s="51"/>
       <c r="L19" s="51"/>
       <c r="M19" s="51"/>
-      <c r="N19" s="123"/>
+      <c r="N19" s="122"/>
       <c r="O19" s="49"/>
       <c r="P19" s="50"/>
       <c r="Q19" s="14"/>
@@ -8985,7 +8978,7 @@
       <c r="K20" s="51"/>
       <c r="L20" s="51"/>
       <c r="M20" s="51"/>
-      <c r="N20" s="123"/>
+      <c r="N20" s="122"/>
       <c r="O20" s="49"/>
       <c r="P20" s="50"/>
       <c r="Q20" s="14"/>
@@ -9027,7 +9020,7 @@
       <c r="K21" s="51"/>
       <c r="L21" s="51"/>
       <c r="M21" s="51"/>
-      <c r="N21" s="123"/>
+      <c r="N21" s="122"/>
       <c r="O21" s="49"/>
       <c r="P21" s="50"/>
       <c r="Q21" s="14"/>
@@ -9069,7 +9062,7 @@
       <c r="K22" s="51"/>
       <c r="L22" s="51"/>
       <c r="M22" s="51"/>
-      <c r="N22" s="123"/>
+      <c r="N22" s="122"/>
       <c r="O22" s="49"/>
       <c r="P22" s="50"/>
       <c r="Q22" s="14"/>
@@ -9111,7 +9104,7 @@
       <c r="K23" s="51"/>
       <c r="L23" s="51"/>
       <c r="M23" s="51"/>
-      <c r="N23" s="123"/>
+      <c r="N23" s="122"/>
       <c r="O23" s="49"/>
       <c r="P23" s="50"/>
       <c r="Q23" s="14"/>
@@ -9153,7 +9146,7 @@
       <c r="K24" s="51"/>
       <c r="L24" s="51"/>
       <c r="M24" s="51"/>
-      <c r="N24" s="123"/>
+      <c r="N24" s="122"/>
       <c r="O24" s="49"/>
       <c r="P24" s="50"/>
       <c r="Q24" s="14"/>
@@ -9195,7 +9188,7 @@
       <c r="K25" s="51"/>
       <c r="L25" s="51"/>
       <c r="M25" s="51"/>
-      <c r="N25" s="123"/>
+      <c r="N25" s="122"/>
       <c r="O25" s="49"/>
       <c r="P25" s="50"/>
       <c r="Q25" s="14"/>
@@ -9237,7 +9230,7 @@
       <c r="K26" s="51"/>
       <c r="L26" s="51"/>
       <c r="M26" s="51"/>
-      <c r="N26" s="123"/>
+      <c r="N26" s="122"/>
       <c r="O26" s="49"/>
       <c r="P26" s="50"/>
       <c r="Q26" s="14"/>
@@ -9279,7 +9272,7 @@
       <c r="K27" s="51"/>
       <c r="L27" s="51"/>
       <c r="M27" s="51"/>
-      <c r="N27" s="123"/>
+      <c r="N27" s="122"/>
       <c r="O27" s="49"/>
       <c r="P27" s="50"/>
       <c r="Q27" s="14"/>
@@ -9321,7 +9314,7 @@
       <c r="K28" s="51"/>
       <c r="L28" s="51"/>
       <c r="M28" s="51"/>
-      <c r="N28" s="123"/>
+      <c r="N28" s="122"/>
       <c r="O28" s="49"/>
       <c r="P28" s="50"/>
       <c r="Q28" s="14"/>
@@ -9363,7 +9356,7 @@
       <c r="K29" s="51"/>
       <c r="L29" s="51"/>
       <c r="M29" s="51"/>
-      <c r="N29" s="123"/>
+      <c r="N29" s="122"/>
       <c r="O29" s="49"/>
       <c r="P29" s="50"/>
       <c r="Q29" s="14"/>
@@ -9405,7 +9398,7 @@
       <c r="K30" s="51"/>
       <c r="L30" s="51"/>
       <c r="M30" s="51"/>
-      <c r="N30" s="123"/>
+      <c r="N30" s="122"/>
       <c r="O30" s="49"/>
       <c r="P30" s="50"/>
       <c r="Q30" s="14"/>
@@ -9447,7 +9440,7 @@
       <c r="K31" s="51"/>
       <c r="L31" s="51"/>
       <c r="M31" s="51"/>
-      <c r="N31" s="123"/>
+      <c r="N31" s="122"/>
       <c r="O31" s="49"/>
       <c r="P31" s="50"/>
       <c r="Q31" s="14"/>
@@ -9489,7 +9482,7 @@
       <c r="K32" s="51"/>
       <c r="L32" s="51"/>
       <c r="M32" s="51"/>
-      <c r="N32" s="123"/>
+      <c r="N32" s="122"/>
       <c r="O32" s="49"/>
       <c r="P32" s="50"/>
       <c r="Q32" s="14"/>
@@ -9531,7 +9524,7 @@
       <c r="K33" s="51"/>
       <c r="L33" s="51"/>
       <c r="M33" s="51"/>
-      <c r="N33" s="123"/>
+      <c r="N33" s="122"/>
       <c r="O33" s="49"/>
       <c r="P33" s="50"/>
       <c r="Q33" s="14"/>
@@ -9573,7 +9566,7 @@
       <c r="K34" s="51"/>
       <c r="L34" s="51"/>
       <c r="M34" s="51"/>
-      <c r="N34" s="123"/>
+      <c r="N34" s="122"/>
       <c r="O34" s="49"/>
       <c r="P34" s="50"/>
       <c r="Q34" s="14"/>
@@ -9615,7 +9608,7 @@
       <c r="K35" s="51"/>
       <c r="L35" s="51"/>
       <c r="M35" s="51"/>
-      <c r="N35" s="123"/>
+      <c r="N35" s="122"/>
       <c r="O35" s="49"/>
       <c r="P35" s="50"/>
       <c r="Q35" s="14"/>
@@ -9657,7 +9650,7 @@
       <c r="K36" s="51"/>
       <c r="L36" s="51"/>
       <c r="M36" s="51"/>
-      <c r="N36" s="123"/>
+      <c r="N36" s="122"/>
       <c r="O36" s="49"/>
       <c r="P36" s="50"/>
       <c r="Q36" s="14"/>
@@ -9699,7 +9692,7 @@
       <c r="K37" s="51"/>
       <c r="L37" s="51"/>
       <c r="M37" s="51"/>
-      <c r="N37" s="123"/>
+      <c r="N37" s="122"/>
       <c r="O37" s="49"/>
       <c r="P37" s="50"/>
       <c r="Q37" s="14"/>
@@ -9741,7 +9734,7 @@
       <c r="K38" s="51"/>
       <c r="L38" s="51"/>
       <c r="M38" s="51"/>
-      <c r="N38" s="123"/>
+      <c r="N38" s="122"/>
       <c r="O38" s="49"/>
       <c r="P38" s="50"/>
       <c r="Q38" s="14"/>
@@ -9783,7 +9776,7 @@
       <c r="K39" s="51"/>
       <c r="L39" s="51"/>
       <c r="M39" s="51"/>
-      <c r="N39" s="123"/>
+      <c r="N39" s="122"/>
       <c r="O39" s="49"/>
       <c r="P39" s="50"/>
       <c r="Q39" s="14"/>
@@ -9825,7 +9818,7 @@
       <c r="K40" s="51"/>
       <c r="L40" s="51"/>
       <c r="M40" s="51"/>
-      <c r="N40" s="123"/>
+      <c r="N40" s="122"/>
       <c r="O40" s="49"/>
       <c r="P40" s="50"/>
       <c r="Q40" s="14"/>
@@ -9867,7 +9860,7 @@
       <c r="K41" s="51"/>
       <c r="L41" s="51"/>
       <c r="M41" s="51"/>
-      <c r="N41" s="123"/>
+      <c r="N41" s="122"/>
       <c r="O41" s="49"/>
       <c r="P41" s="50"/>
       <c r="Q41" s="14"/>
@@ -9909,7 +9902,7 @@
       <c r="K42" s="51"/>
       <c r="L42" s="51"/>
       <c r="M42" s="51"/>
-      <c r="N42" s="123"/>
+      <c r="N42" s="122"/>
       <c r="O42" s="49"/>
       <c r="P42" s="50"/>
       <c r="Q42" s="14"/>
@@ -9951,7 +9944,7 @@
       <c r="K43" s="51"/>
       <c r="L43" s="51"/>
       <c r="M43" s="51"/>
-      <c r="N43" s="123"/>
+      <c r="N43" s="122"/>
       <c r="O43" s="49"/>
       <c r="P43" s="50"/>
       <c r="Q43" s="14"/>
@@ -9993,7 +9986,7 @@
       <c r="K44" s="51"/>
       <c r="L44" s="51"/>
       <c r="M44" s="51"/>
-      <c r="N44" s="123"/>
+      <c r="N44" s="122"/>
       <c r="O44" s="49"/>
       <c r="P44" s="50"/>
       <c r="Q44" s="14"/>
@@ -10035,7 +10028,7 @@
       <c r="K45" s="51"/>
       <c r="L45" s="51"/>
       <c r="M45" s="51"/>
-      <c r="N45" s="123"/>
+      <c r="N45" s="122"/>
       <c r="O45" s="49"/>
       <c r="P45" s="50"/>
       <c r="Q45" s="14"/>
@@ -10077,7 +10070,7 @@
       <c r="K46" s="51"/>
       <c r="L46" s="51"/>
       <c r="M46" s="51"/>
-      <c r="N46" s="123"/>
+      <c r="N46" s="122"/>
       <c r="O46" s="49"/>
       <c r="P46" s="50"/>
       <c r="Q46" s="14"/>
@@ -10119,7 +10112,7 @@
       <c r="K47" s="51"/>
       <c r="L47" s="51"/>
       <c r="M47" s="51"/>
-      <c r="N47" s="123"/>
+      <c r="N47" s="122"/>
       <c r="O47" s="49"/>
       <c r="P47" s="50"/>
       <c r="Q47" s="14"/>
@@ -10161,7 +10154,7 @@
       <c r="K48" s="51"/>
       <c r="L48" s="51"/>
       <c r="M48" s="51"/>
-      <c r="N48" s="123"/>
+      <c r="N48" s="122"/>
       <c r="O48" s="49"/>
       <c r="P48" s="50"/>
       <c r="Q48" s="14"/>
@@ -10203,7 +10196,7 @@
       <c r="K49" s="51"/>
       <c r="L49" s="51"/>
       <c r="M49" s="51"/>
-      <c r="N49" s="123"/>
+      <c r="N49" s="122"/>
       <c r="O49" s="49"/>
       <c r="P49" s="50"/>
       <c r="Q49" s="14"/>
@@ -10245,7 +10238,7 @@
       <c r="K50" s="51"/>
       <c r="L50" s="51"/>
       <c r="M50" s="51"/>
-      <c r="N50" s="123"/>
+      <c r="N50" s="122"/>
       <c r="O50" s="49"/>
       <c r="P50" s="50"/>
       <c r="Q50" s="14"/>
@@ -10287,7 +10280,7 @@
       <c r="K51" s="51"/>
       <c r="L51" s="51"/>
       <c r="M51" s="51"/>
-      <c r="N51" s="123"/>
+      <c r="N51" s="122"/>
       <c r="O51" s="49"/>
       <c r="P51" s="50"/>
       <c r="Q51" s="14"/>
@@ -10329,7 +10322,7 @@
       <c r="K52" s="51"/>
       <c r="L52" s="51"/>
       <c r="M52" s="51"/>
-      <c r="N52" s="123"/>
+      <c r="N52" s="122"/>
       <c r="O52" s="49"/>
       <c r="P52" s="50"/>
       <c r="Q52" s="14"/>
@@ -10371,7 +10364,7 @@
       <c r="K53" s="51"/>
       <c r="L53" s="51"/>
       <c r="M53" s="51"/>
-      <c r="N53" s="123"/>
+      <c r="N53" s="122"/>
       <c r="O53" s="49"/>
       <c r="P53" s="50"/>
       <c r="Q53" s="14"/>
@@ -10413,7 +10406,7 @@
       <c r="K54" s="51"/>
       <c r="L54" s="51"/>
       <c r="M54" s="51"/>
-      <c r="N54" s="123"/>
+      <c r="N54" s="122"/>
       <c r="O54" s="49"/>
       <c r="P54" s="50"/>
       <c r="Q54" s="14"/>
@@ -10455,7 +10448,7 @@
       <c r="K55" s="51"/>
       <c r="L55" s="51"/>
       <c r="M55" s="51"/>
-      <c r="N55" s="123"/>
+      <c r="N55" s="122"/>
       <c r="O55" s="49"/>
       <c r="P55" s="50"/>
       <c r="Q55" s="14"/>
@@ -10497,7 +10490,7 @@
       <c r="K56" s="51"/>
       <c r="L56" s="51"/>
       <c r="M56" s="51"/>
-      <c r="N56" s="123"/>
+      <c r="N56" s="122"/>
       <c r="O56" s="49"/>
       <c r="P56" s="50"/>
       <c r="Q56" s="14"/>
@@ -10539,7 +10532,7 @@
       <c r="K57" s="51"/>
       <c r="L57" s="51"/>
       <c r="M57" s="51"/>
-      <c r="N57" s="123"/>
+      <c r="N57" s="122"/>
       <c r="O57" s="49"/>
       <c r="P57" s="50"/>
       <c r="Q57" s="14"/>
@@ -10581,7 +10574,7 @@
       <c r="K58" s="51"/>
       <c r="L58" s="51"/>
       <c r="M58" s="51"/>
-      <c r="N58" s="123"/>
+      <c r="N58" s="122"/>
       <c r="O58" s="49"/>
       <c r="P58" s="50"/>
       <c r="Q58" s="14"/>
@@ -10623,7 +10616,7 @@
       <c r="K59" s="51"/>
       <c r="L59" s="51"/>
       <c r="M59" s="51"/>
-      <c r="N59" s="123"/>
+      <c r="N59" s="122"/>
       <c r="O59" s="49"/>
       <c r="P59" s="50"/>
       <c r="Q59" s="14"/>
@@ -10665,7 +10658,7 @@
       <c r="K60" s="51"/>
       <c r="L60" s="51"/>
       <c r="M60" s="51"/>
-      <c r="N60" s="123"/>
+      <c r="N60" s="122"/>
       <c r="O60" s="49"/>
       <c r="P60" s="50"/>
       <c r="Q60" s="14"/>
@@ -10707,7 +10700,7 @@
       <c r="K61" s="51"/>
       <c r="L61" s="51"/>
       <c r="M61" s="51"/>
-      <c r="N61" s="123"/>
+      <c r="N61" s="122"/>
       <c r="O61" s="49"/>
       <c r="P61" s="50"/>
       <c r="Q61" s="14"/>
@@ -10749,7 +10742,7 @@
       <c r="K62" s="51"/>
       <c r="L62" s="51"/>
       <c r="M62" s="51"/>
-      <c r="N62" s="123"/>
+      <c r="N62" s="122"/>
       <c r="O62" s="49"/>
       <c r="P62" s="50"/>
       <c r="Q62" s="14"/>
@@ -10791,7 +10784,7 @@
       <c r="K63" s="51"/>
       <c r="L63" s="51"/>
       <c r="M63" s="51"/>
-      <c r="N63" s="123"/>
+      <c r="N63" s="122"/>
       <c r="O63" s="49"/>
       <c r="P63" s="50"/>
       <c r="Q63" s="14"/>
@@ -10833,7 +10826,7 @@
       <c r="K64" s="51"/>
       <c r="L64" s="51"/>
       <c r="M64" s="51"/>
-      <c r="N64" s="123"/>
+      <c r="N64" s="122"/>
       <c r="O64" s="49"/>
       <c r="P64" s="50"/>
       <c r="Q64" s="14"/>
@@ -10875,7 +10868,7 @@
       <c r="K65" s="51"/>
       <c r="L65" s="51"/>
       <c r="M65" s="51"/>
-      <c r="N65" s="123"/>
+      <c r="N65" s="122"/>
       <c r="O65" s="49"/>
       <c r="P65" s="50"/>
       <c r="Q65" s="14"/>
@@ -10917,7 +10910,7 @@
       <c r="K66" s="51"/>
       <c r="L66" s="51"/>
       <c r="M66" s="51"/>
-      <c r="N66" s="123"/>
+      <c r="N66" s="122"/>
       <c r="O66" s="49"/>
       <c r="P66" s="50"/>
       <c r="Q66" s="14"/>
@@ -10959,7 +10952,7 @@
       <c r="K67" s="51"/>
       <c r="L67" s="51"/>
       <c r="M67" s="51"/>
-      <c r="N67" s="123"/>
+      <c r="N67" s="122"/>
       <c r="O67" s="49"/>
       <c r="P67" s="50"/>
       <c r="Q67" s="14"/>
@@ -11001,7 +10994,7 @@
       <c r="K68" s="51"/>
       <c r="L68" s="51"/>
       <c r="M68" s="51"/>
-      <c r="N68" s="123"/>
+      <c r="N68" s="122"/>
       <c r="O68" s="49"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="14"/>
@@ -11043,7 +11036,7 @@
       <c r="K69" s="51"/>
       <c r="L69" s="51"/>
       <c r="M69" s="51"/>
-      <c r="N69" s="123"/>
+      <c r="N69" s="122"/>
       <c r="O69" s="49"/>
       <c r="P69" s="50"/>
       <c r="Q69" s="14"/>
@@ -11085,7 +11078,7 @@
       <c r="K70" s="51"/>
       <c r="L70" s="51"/>
       <c r="M70" s="51"/>
-      <c r="N70" s="123"/>
+      <c r="N70" s="122"/>
       <c r="O70" s="49"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="14"/>
@@ -11127,7 +11120,7 @@
       <c r="K71" s="51"/>
       <c r="L71" s="51"/>
       <c r="M71" s="51"/>
-      <c r="N71" s="123"/>
+      <c r="N71" s="122"/>
       <c r="O71" s="49"/>
       <c r="P71" s="50"/>
       <c r="Q71" s="14"/>
@@ -11169,7 +11162,7 @@
       <c r="K72" s="51"/>
       <c r="L72" s="51"/>
       <c r="M72" s="51"/>
-      <c r="N72" s="123"/>
+      <c r="N72" s="122"/>
       <c r="O72" s="49"/>
       <c r="P72" s="50"/>
       <c r="Q72" s="14"/>
@@ -11211,7 +11204,7 @@
       <c r="K73" s="51"/>
       <c r="L73" s="51"/>
       <c r="M73" s="51"/>
-      <c r="N73" s="123"/>
+      <c r="N73" s="122"/>
       <c r="O73" s="49"/>
       <c r="P73" s="50"/>
       <c r="Q73" s="14"/>
@@ -11253,7 +11246,7 @@
       <c r="K74" s="51"/>
       <c r="L74" s="51"/>
       <c r="M74" s="51"/>
-      <c r="N74" s="123"/>
+      <c r="N74" s="122"/>
       <c r="O74" s="49"/>
       <c r="P74" s="50"/>
       <c r="Q74" s="14"/>
@@ -11295,7 +11288,7 @@
       <c r="K75" s="51"/>
       <c r="L75" s="51"/>
       <c r="M75" s="51"/>
-      <c r="N75" s="123"/>
+      <c r="N75" s="122"/>
       <c r="O75" s="49"/>
       <c r="P75" s="50"/>
       <c r="Q75" s="14"/>
@@ -11337,7 +11330,7 @@
       <c r="K76" s="51"/>
       <c r="L76" s="51"/>
       <c r="M76" s="51"/>
-      <c r="N76" s="123"/>
+      <c r="N76" s="122"/>
       <c r="O76" s="49"/>
       <c r="P76" s="50"/>
       <c r="Q76" s="14"/>
@@ -11379,7 +11372,7 @@
       <c r="K77" s="51"/>
       <c r="L77" s="51"/>
       <c r="M77" s="51"/>
-      <c r="N77" s="123"/>
+      <c r="N77" s="122"/>
       <c r="O77" s="49"/>
       <c r="P77" s="50"/>
       <c r="Q77" s="14"/>
@@ -11421,7 +11414,7 @@
       <c r="K78" s="51"/>
       <c r="L78" s="51"/>
       <c r="M78" s="51"/>
-      <c r="N78" s="123"/>
+      <c r="N78" s="122"/>
       <c r="O78" s="49"/>
       <c r="P78" s="50"/>
       <c r="Q78" s="14"/>
@@ -11463,7 +11456,7 @@
       <c r="K79" s="51"/>
       <c r="L79" s="51"/>
       <c r="M79" s="51"/>
-      <c r="N79" s="123"/>
+      <c r="N79" s="122"/>
       <c r="O79" s="49"/>
       <c r="P79" s="50"/>
       <c r="Q79" s="14"/>
@@ -11505,7 +11498,7 @@
       <c r="K80" s="51"/>
       <c r="L80" s="51"/>
       <c r="M80" s="51"/>
-      <c r="N80" s="123"/>
+      <c r="N80" s="122"/>
       <c r="O80" s="49"/>
       <c r="P80" s="50"/>
       <c r="Q80" s="14"/>
@@ -11547,7 +11540,7 @@
       <c r="K81" s="51"/>
       <c r="L81" s="51"/>
       <c r="M81" s="51"/>
-      <c r="N81" s="123"/>
+      <c r="N81" s="122"/>
       <c r="O81" s="49"/>
       <c r="P81" s="50"/>
       <c r="Q81" s="14"/>
@@ -11589,7 +11582,7 @@
       <c r="K82" s="51"/>
       <c r="L82" s="51"/>
       <c r="M82" s="51"/>
-      <c r="N82" s="123"/>
+      <c r="N82" s="122"/>
       <c r="O82" s="49"/>
       <c r="P82" s="50"/>
       <c r="Q82" s="14"/>
@@ -11631,7 +11624,7 @@
       <c r="K83" s="51"/>
       <c r="L83" s="51"/>
       <c r="M83" s="51"/>
-      <c r="N83" s="123"/>
+      <c r="N83" s="122"/>
       <c r="O83" s="49"/>
       <c r="P83" s="50"/>
       <c r="Q83" s="14"/>
@@ -11673,7 +11666,7 @@
       <c r="K84" s="51"/>
       <c r="L84" s="51"/>
       <c r="M84" s="51"/>
-      <c r="N84" s="123"/>
+      <c r="N84" s="122"/>
       <c r="O84" s="49"/>
       <c r="P84" s="50"/>
       <c r="Q84" s="14"/>
@@ -11715,7 +11708,7 @@
       <c r="K85" s="51"/>
       <c r="L85" s="51"/>
       <c r="M85" s="51"/>
-      <c r="N85" s="123"/>
+      <c r="N85" s="122"/>
       <c r="O85" s="49"/>
       <c r="P85" s="50"/>
       <c r="Q85" s="14"/>
@@ -11757,7 +11750,7 @@
       <c r="K86" s="51"/>
       <c r="L86" s="51"/>
       <c r="M86" s="51"/>
-      <c r="N86" s="123"/>
+      <c r="N86" s="122"/>
       <c r="O86" s="49"/>
       <c r="P86" s="50"/>
       <c r="Q86" s="14"/>
@@ -11799,7 +11792,7 @@
       <c r="K87" s="51"/>
       <c r="L87" s="51"/>
       <c r="M87" s="51"/>
-      <c r="N87" s="123"/>
+      <c r="N87" s="122"/>
       <c r="O87" s="49"/>
       <c r="P87" s="50"/>
       <c r="Q87" s="14"/>
@@ -11841,7 +11834,7 @@
       <c r="K88" s="51"/>
       <c r="L88" s="51"/>
       <c r="M88" s="51"/>
-      <c r="N88" s="123"/>
+      <c r="N88" s="122"/>
       <c r="O88" s="49"/>
       <c r="P88" s="50"/>
       <c r="Q88" s="14"/>
@@ -11883,7 +11876,7 @@
       <c r="K89" s="51"/>
       <c r="L89" s="51"/>
       <c r="M89" s="51"/>
-      <c r="N89" s="123"/>
+      <c r="N89" s="122"/>
       <c r="O89" s="49"/>
       <c r="P89" s="50"/>
       <c r="Q89" s="14"/>
@@ -11925,7 +11918,7 @@
       <c r="K90" s="51"/>
       <c r="L90" s="51"/>
       <c r="M90" s="51"/>
-      <c r="N90" s="123"/>
+      <c r="N90" s="122"/>
       <c r="O90" s="49"/>
       <c r="P90" s="50"/>
       <c r="Q90" s="14"/>
@@ -11967,7 +11960,7 @@
       <c r="K91" s="51"/>
       <c r="L91" s="51"/>
       <c r="M91" s="51"/>
-      <c r="N91" s="123"/>
+      <c r="N91" s="122"/>
       <c r="O91" s="49"/>
       <c r="P91" s="50"/>
       <c r="Q91" s="14"/>
@@ -12009,7 +12002,7 @@
       <c r="K92" s="51"/>
       <c r="L92" s="51"/>
       <c r="M92" s="51"/>
-      <c r="N92" s="123"/>
+      <c r="N92" s="122"/>
       <c r="O92" s="49"/>
       <c r="P92" s="50"/>
       <c r="Q92" s="14"/>
@@ -12051,7 +12044,7 @@
       <c r="K93" s="51"/>
       <c r="L93" s="51"/>
       <c r="M93" s="51"/>
-      <c r="N93" s="123"/>
+      <c r="N93" s="122"/>
       <c r="O93" s="49"/>
       <c r="P93" s="50"/>
       <c r="Q93" s="14"/>
@@ -12093,7 +12086,7 @@
       <c r="K94" s="51"/>
       <c r="L94" s="51"/>
       <c r="M94" s="51"/>
-      <c r="N94" s="123"/>
+      <c r="N94" s="122"/>
       <c r="O94" s="49"/>
       <c r="P94" s="50"/>
       <c r="Q94" s="14"/>
@@ -12135,7 +12128,7 @@
       <c r="K95" s="51"/>
       <c r="L95" s="51"/>
       <c r="M95" s="51"/>
-      <c r="N95" s="123"/>
+      <c r="N95" s="122"/>
       <c r="O95" s="49"/>
       <c r="P95" s="50"/>
       <c r="Q95" s="14"/>
@@ -12177,7 +12170,7 @@
       <c r="K96" s="51"/>
       <c r="L96" s="51"/>
       <c r="M96" s="51"/>
-      <c r="N96" s="123"/>
+      <c r="N96" s="122"/>
       <c r="O96" s="49"/>
       <c r="P96" s="50"/>
       <c r="Q96" s="14"/>
@@ -12219,7 +12212,7 @@
       <c r="K97" s="51"/>
       <c r="L97" s="51"/>
       <c r="M97" s="51"/>
-      <c r="N97" s="123"/>
+      <c r="N97" s="122"/>
       <c r="O97" s="49"/>
       <c r="P97" s="50"/>
       <c r="Q97" s="14"/>
@@ -12261,7 +12254,7 @@
       <c r="K98" s="51"/>
       <c r="L98" s="51"/>
       <c r="M98" s="51"/>
-      <c r="N98" s="123"/>
+      <c r="N98" s="122"/>
       <c r="O98" s="49"/>
       <c r="P98" s="50"/>
       <c r="Q98" s="14"/>
@@ -12303,7 +12296,7 @@
       <c r="K99" s="51"/>
       <c r="L99" s="51"/>
       <c r="M99" s="51"/>
-      <c r="N99" s="123"/>
+      <c r="N99" s="122"/>
       <c r="O99" s="49"/>
       <c r="P99" s="50"/>
       <c r="Q99" s="14"/>
@@ -12345,7 +12338,7 @@
       <c r="K100" s="51"/>
       <c r="L100" s="51"/>
       <c r="M100" s="51"/>
-      <c r="N100" s="123"/>
+      <c r="N100" s="122"/>
       <c r="O100" s="49"/>
       <c r="P100" s="50"/>
       <c r="Q100" s="14"/>
@@ -12387,7 +12380,7 @@
       <c r="K101" s="51"/>
       <c r="L101" s="51"/>
       <c r="M101" s="51"/>
-      <c r="N101" s="123"/>
+      <c r="N101" s="122"/>
       <c r="O101" s="49"/>
       <c r="P101" s="50"/>
       <c r="Q101" s="14"/>
@@ -12429,7 +12422,7 @@
       <c r="K102" s="51"/>
       <c r="L102" s="51"/>
       <c r="M102" s="51"/>
-      <c r="N102" s="123"/>
+      <c r="N102" s="122"/>
       <c r="O102" s="49"/>
       <c r="P102" s="50"/>
       <c r="Q102" s="14"/>
@@ -12471,7 +12464,7 @@
       <c r="K103" s="51"/>
       <c r="L103" s="51"/>
       <c r="M103" s="51"/>
-      <c r="N103" s="123"/>
+      <c r="N103" s="122"/>
       <c r="O103" s="49"/>
       <c r="P103" s="50"/>
       <c r="Q103" s="14"/>
@@ -12513,7 +12506,7 @@
       <c r="K104" s="51"/>
       <c r="L104" s="51"/>
       <c r="M104" s="51"/>
-      <c r="N104" s="123"/>
+      <c r="N104" s="122"/>
       <c r="O104" s="49"/>
       <c r="P104" s="50"/>
       <c r="Q104" s="14"/>
@@ -12555,7 +12548,7 @@
       <c r="K105" s="51"/>
       <c r="L105" s="51"/>
       <c r="M105" s="51"/>
-      <c r="N105" s="123"/>
+      <c r="N105" s="122"/>
       <c r="O105" s="49"/>
       <c r="P105" s="50"/>
       <c r="Q105" s="14"/>
@@ -12597,7 +12590,7 @@
       <c r="K106" s="51"/>
       <c r="L106" s="51"/>
       <c r="M106" s="51"/>
-      <c r="N106" s="123"/>
+      <c r="N106" s="122"/>
       <c r="O106" s="49"/>
       <c r="P106" s="50"/>
       <c r="Q106" s="14"/>
@@ -12639,7 +12632,7 @@
       <c r="K107" s="51"/>
       <c r="L107" s="51"/>
       <c r="M107" s="51"/>
-      <c r="N107" s="123"/>
+      <c r="N107" s="122"/>
       <c r="O107" s="49"/>
       <c r="P107" s="50"/>
       <c r="Q107" s="14"/>
@@ -12681,7 +12674,7 @@
       <c r="K108" s="51"/>
       <c r="L108" s="51"/>
       <c r="M108" s="51"/>
-      <c r="N108" s="123"/>
+      <c r="N108" s="122"/>
       <c r="O108" s="49"/>
       <c r="P108" s="50"/>
       <c r="Q108" s="14"/>
@@ -12723,7 +12716,7 @@
       <c r="K109" s="51"/>
       <c r="L109" s="51"/>
       <c r="M109" s="51"/>
-      <c r="N109" s="123"/>
+      <c r="N109" s="122"/>
       <c r="O109" s="49"/>
       <c r="P109" s="50"/>
       <c r="Q109" s="14"/>
@@ -12765,7 +12758,7 @@
       <c r="K110" s="51"/>
       <c r="L110" s="51"/>
       <c r="M110" s="51"/>
-      <c r="N110" s="123"/>
+      <c r="N110" s="122"/>
       <c r="O110" s="49"/>
       <c r="P110" s="50"/>
       <c r="Q110" s="14"/>
@@ -12807,7 +12800,7 @@
       <c r="K111" s="51"/>
       <c r="L111" s="51"/>
       <c r="M111" s="51"/>
-      <c r="N111" s="123"/>
+      <c r="N111" s="122"/>
       <c r="O111" s="49"/>
       <c r="P111" s="50"/>
       <c r="Q111" s="14"/>
@@ -12849,7 +12842,7 @@
       <c r="K112" s="51"/>
       <c r="L112" s="51"/>
       <c r="M112" s="51"/>
-      <c r="N112" s="123"/>
+      <c r="N112" s="122"/>
       <c r="O112" s="49"/>
       <c r="P112" s="50"/>
       <c r="Q112" s="14"/>
@@ -12891,7 +12884,7 @@
       <c r="K113" s="51"/>
       <c r="L113" s="51"/>
       <c r="M113" s="51"/>
-      <c r="N113" s="123"/>
+      <c r="N113" s="122"/>
       <c r="O113" s="49"/>
       <c r="P113" s="50"/>
       <c r="Q113" s="14"/>
@@ -12933,7 +12926,7 @@
       <c r="K114" s="51"/>
       <c r="L114" s="51"/>
       <c r="M114" s="51"/>
-      <c r="N114" s="123"/>
+      <c r="N114" s="122"/>
       <c r="O114" s="49"/>
       <c r="P114" s="50"/>
       <c r="Q114" s="14"/>
@@ -12975,7 +12968,7 @@
       <c r="K115" s="51"/>
       <c r="L115" s="51"/>
       <c r="M115" s="51"/>
-      <c r="N115" s="123"/>
+      <c r="N115" s="122"/>
       <c r="O115" s="49"/>
       <c r="P115" s="50"/>
       <c r="Q115" s="14"/>
@@ -13017,7 +13010,7 @@
       <c r="K116" s="51"/>
       <c r="L116" s="51"/>
       <c r="M116" s="51"/>
-      <c r="N116" s="123"/>
+      <c r="N116" s="122"/>
       <c r="O116" s="49"/>
       <c r="P116" s="50"/>
       <c r="Q116" s="14"/>
@@ -13059,7 +13052,7 @@
       <c r="K117" s="51"/>
       <c r="L117" s="51"/>
       <c r="M117" s="51"/>
-      <c r="N117" s="123"/>
+      <c r="N117" s="122"/>
       <c r="O117" s="49"/>
       <c r="P117" s="50"/>
       <c r="Q117" s="14"/>
@@ -13101,7 +13094,7 @@
       <c r="K118" s="51"/>
       <c r="L118" s="51"/>
       <c r="M118" s="51"/>
-      <c r="N118" s="123"/>
+      <c r="N118" s="122"/>
       <c r="O118" s="49"/>
       <c r="P118" s="50"/>
       <c r="Q118" s="14"/>
@@ -13143,7 +13136,7 @@
       <c r="K119" s="51"/>
       <c r="L119" s="51"/>
       <c r="M119" s="51"/>
-      <c r="N119" s="123"/>
+      <c r="N119" s="122"/>
       <c r="O119" s="49"/>
       <c r="P119" s="50"/>
       <c r="Q119" s="14"/>
@@ -13185,7 +13178,7 @@
       <c r="K120" s="51"/>
       <c r="L120" s="51"/>
       <c r="M120" s="51"/>
-      <c r="N120" s="123"/>
+      <c r="N120" s="122"/>
       <c r="O120" s="49"/>
       <c r="P120" s="50"/>
       <c r="Q120" s="14"/>
@@ -13227,7 +13220,7 @@
       <c r="K121" s="51"/>
       <c r="L121" s="51"/>
       <c r="M121" s="51"/>
-      <c r="N121" s="123"/>
+      <c r="N121" s="122"/>
       <c r="O121" s="49"/>
       <c r="P121" s="50"/>
       <c r="Q121" s="14"/>
@@ -13269,7 +13262,7 @@
       <c r="K122" s="51"/>
       <c r="L122" s="51"/>
       <c r="M122" s="51"/>
-      <c r="N122" s="123"/>
+      <c r="N122" s="122"/>
       <c r="O122" s="49"/>
       <c r="P122" s="50"/>
       <c r="Q122" s="14"/>
@@ -13311,7 +13304,7 @@
       <c r="K123" s="51"/>
       <c r="L123" s="51"/>
       <c r="M123" s="51"/>
-      <c r="N123" s="123"/>
+      <c r="N123" s="122"/>
       <c r="O123" s="49"/>
       <c r="P123" s="50"/>
       <c r="Q123" s="14"/>
@@ -13353,7 +13346,7 @@
       <c r="K124" s="51"/>
       <c r="L124" s="51"/>
       <c r="M124" s="51"/>
-      <c r="N124" s="123"/>
+      <c r="N124" s="122"/>
       <c r="O124" s="49"/>
       <c r="P124" s="50"/>
       <c r="Q124" s="14"/>
@@ -13395,7 +13388,7 @@
       <c r="K125" s="51"/>
       <c r="L125" s="51"/>
       <c r="M125" s="51"/>
-      <c r="N125" s="123"/>
+      <c r="N125" s="122"/>
       <c r="O125" s="49"/>
       <c r="P125" s="50"/>
       <c r="Q125" s="14"/>
@@ -13437,7 +13430,7 @@
       <c r="K126" s="51"/>
       <c r="L126" s="51"/>
       <c r="M126" s="51"/>
-      <c r="N126" s="123"/>
+      <c r="N126" s="122"/>
       <c r="O126" s="49"/>
       <c r="P126" s="50"/>
       <c r="Q126" s="14"/>
@@ -13479,7 +13472,7 @@
       <c r="K127" s="51"/>
       <c r="L127" s="51"/>
       <c r="M127" s="51"/>
-      <c r="N127" s="123"/>
+      <c r="N127" s="122"/>
       <c r="O127" s="49"/>
       <c r="P127" s="50"/>
       <c r="Q127" s="14"/>
@@ -13521,7 +13514,7 @@
       <c r="K128" s="51"/>
       <c r="L128" s="51"/>
       <c r="M128" s="51"/>
-      <c r="N128" s="123"/>
+      <c r="N128" s="122"/>
       <c r="O128" s="49"/>
       <c r="P128" s="50"/>
       <c r="Q128" s="14"/>
@@ -13563,7 +13556,7 @@
       <c r="K129" s="51"/>
       <c r="L129" s="51"/>
       <c r="M129" s="51"/>
-      <c r="N129" s="123"/>
+      <c r="N129" s="122"/>
       <c r="O129" s="49"/>
       <c r="P129" s="50"/>
       <c r="Q129" s="14"/>
@@ -13605,7 +13598,7 @@
       <c r="K130" s="51"/>
       <c r="L130" s="51"/>
       <c r="M130" s="51"/>
-      <c r="N130" s="123"/>
+      <c r="N130" s="122"/>
       <c r="O130" s="49"/>
       <c r="P130" s="50"/>
       <c r="Q130" s="14"/>
@@ -13647,7 +13640,7 @@
       <c r="K131" s="51"/>
       <c r="L131" s="51"/>
       <c r="M131" s="51"/>
-      <c r="N131" s="123"/>
+      <c r="N131" s="122"/>
       <c r="O131" s="49"/>
       <c r="P131" s="50"/>
       <c r="Q131" s="14"/>
@@ -13689,7 +13682,7 @@
       <c r="K132" s="51"/>
       <c r="L132" s="51"/>
       <c r="M132" s="51"/>
-      <c r="N132" s="123"/>
+      <c r="N132" s="122"/>
       <c r="O132" s="49"/>
       <c r="P132" s="50"/>
       <c r="Q132" s="14"/>
@@ -13731,7 +13724,7 @@
       <c r="K133" s="51"/>
       <c r="L133" s="51"/>
       <c r="M133" s="51"/>
-      <c r="N133" s="123"/>
+      <c r="N133" s="122"/>
       <c r="O133" s="49"/>
       <c r="P133" s="50"/>
       <c r="Q133" s="14"/>
@@ -13773,7 +13766,7 @@
       <c r="K134" s="51"/>
       <c r="L134" s="51"/>
       <c r="M134" s="51"/>
-      <c r="N134" s="123"/>
+      <c r="N134" s="122"/>
       <c r="O134" s="49"/>
       <c r="P134" s="50"/>
       <c r="Q134" s="14"/>
@@ -13815,7 +13808,7 @@
       <c r="K135" s="51"/>
       <c r="L135" s="51"/>
       <c r="M135" s="51"/>
-      <c r="N135" s="123"/>
+      <c r="N135" s="122"/>
       <c r="O135" s="49"/>
       <c r="P135" s="50"/>
       <c r="Q135" s="14"/>
@@ -13857,7 +13850,7 @@
       <c r="K136" s="51"/>
       <c r="L136" s="51"/>
       <c r="M136" s="51"/>
-      <c r="N136" s="123"/>
+      <c r="N136" s="122"/>
       <c r="O136" s="49"/>
       <c r="P136" s="50"/>
       <c r="Q136" s="14"/>
@@ -13899,7 +13892,7 @@
       <c r="K137" s="51"/>
       <c r="L137" s="51"/>
       <c r="M137" s="51"/>
-      <c r="N137" s="123"/>
+      <c r="N137" s="122"/>
       <c r="O137" s="49"/>
       <c r="P137" s="50"/>
       <c r="Q137" s="14"/>
@@ -13941,7 +13934,7 @@
       <c r="K138" s="51"/>
       <c r="L138" s="51"/>
       <c r="M138" s="51"/>
-      <c r="N138" s="123"/>
+      <c r="N138" s="122"/>
       <c r="O138" s="49"/>
       <c r="P138" s="50"/>
       <c r="Q138" s="14"/>
@@ -13983,7 +13976,7 @@
       <c r="K139" s="51"/>
       <c r="L139" s="51"/>
       <c r="M139" s="51"/>
-      <c r="N139" s="123"/>
+      <c r="N139" s="122"/>
       <c r="O139" s="49"/>
       <c r="P139" s="50"/>
       <c r="Q139" s="14"/>
@@ -14025,7 +14018,7 @@
       <c r="K140" s="51"/>
       <c r="L140" s="51"/>
       <c r="M140" s="51"/>
-      <c r="N140" s="123"/>
+      <c r="N140" s="122"/>
       <c r="O140" s="49"/>
       <c r="P140" s="50"/>
       <c r="Q140" s="14"/>
@@ -14067,7 +14060,7 @@
       <c r="K141" s="51"/>
       <c r="L141" s="51"/>
       <c r="M141" s="51"/>
-      <c r="N141" s="123"/>
+      <c r="N141" s="122"/>
       <c r="O141" s="49"/>
       <c r="P141" s="50"/>
       <c r="Q141" s="14"/>
@@ -14109,7 +14102,7 @@
       <c r="K142" s="51"/>
       <c r="L142" s="51"/>
       <c r="M142" s="51"/>
-      <c r="N142" s="123"/>
+      <c r="N142" s="122"/>
       <c r="O142" s="49"/>
       <c r="P142" s="50"/>
       <c r="Q142" s="14"/>
@@ -14151,7 +14144,7 @@
       <c r="K143" s="51"/>
       <c r="L143" s="51"/>
       <c r="M143" s="51"/>
-      <c r="N143" s="123"/>
+      <c r="N143" s="122"/>
       <c r="O143" s="49"/>
       <c r="P143" s="50"/>
       <c r="Q143" s="14"/>
@@ -14193,7 +14186,7 @@
       <c r="K144" s="51"/>
       <c r="L144" s="51"/>
       <c r="M144" s="51"/>
-      <c r="N144" s="123"/>
+      <c r="N144" s="122"/>
       <c r="O144" s="49"/>
       <c r="P144" s="50"/>
       <c r="Q144" s="14"/>
@@ -14235,7 +14228,7 @@
       <c r="K145" s="51"/>
       <c r="L145" s="51"/>
       <c r="M145" s="51"/>
-      <c r="N145" s="123"/>
+      <c r="N145" s="122"/>
       <c r="O145" s="49"/>
       <c r="P145" s="50"/>
       <c r="Q145" s="14"/>
@@ -14277,7 +14270,7 @@
       <c r="K146" s="51"/>
       <c r="L146" s="51"/>
       <c r="M146" s="51"/>
-      <c r="N146" s="123"/>
+      <c r="N146" s="122"/>
       <c r="O146" s="49"/>
       <c r="P146" s="50"/>
       <c r="Q146" s="14"/>
@@ -14319,7 +14312,7 @@
       <c r="K147" s="51"/>
       <c r="L147" s="51"/>
       <c r="M147" s="51"/>
-      <c r="N147" s="123"/>
+      <c r="N147" s="122"/>
       <c r="O147" s="49"/>
       <c r="P147" s="50"/>
       <c r="Q147" s="14"/>
@@ -14361,7 +14354,7 @@
       <c r="K148" s="51"/>
       <c r="L148" s="51"/>
       <c r="M148" s="51"/>
-      <c r="N148" s="123"/>
+      <c r="N148" s="122"/>
       <c r="O148" s="49"/>
       <c r="P148" s="50"/>
       <c r="Q148" s="14"/>
@@ -14403,7 +14396,7 @@
       <c r="K149" s="51"/>
       <c r="L149" s="51"/>
       <c r="M149" s="51"/>
-      <c r="N149" s="123"/>
+      <c r="N149" s="122"/>
       <c r="O149" s="49"/>
       <c r="P149" s="50"/>
       <c r="Q149" s="14"/>
@@ -14445,7 +14438,7 @@
       <c r="K150" s="51"/>
       <c r="L150" s="51"/>
       <c r="M150" s="51"/>
-      <c r="N150" s="123"/>
+      <c r="N150" s="122"/>
       <c r="O150" s="49"/>
       <c r="P150" s="50"/>
       <c r="Q150" s="14"/>
@@ -47666,20 +47659,6 @@
   <sheetProtection selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="30">
-    <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="AI13:AI14"/>
-    <mergeCell ref="AJ13:AJ14"/>
-    <mergeCell ref="AK13:AK14"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="AD13:AD14"/>
-    <mergeCell ref="AE13:AE14"/>
-    <mergeCell ref="AF13:AF14"/>
-    <mergeCell ref="AG13:AG14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="AH13:AH14"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="AF6:AH6"/>
     <mergeCell ref="A5:F5"/>
@@ -47696,14 +47675,27 @@
     <mergeCell ref="Y13:Y14"/>
     <mergeCell ref="Z13:Z14"/>
     <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="AI13:AI14"/>
+    <mergeCell ref="AJ13:AJ14"/>
+    <mergeCell ref="AK13:AK14"/>
+    <mergeCell ref="AC13:AC14"/>
+    <mergeCell ref="AD13:AD14"/>
+    <mergeCell ref="AE13:AE14"/>
+    <mergeCell ref="AF13:AF14"/>
+    <mergeCell ref="AG13:AG14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="AH13:AH14"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list" sqref="N151" xr:uid="{BB65F868-0ACC-C246-89D1-E55DF7794A56}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" prompt="Click and enter a value from list" sqref="X15:X150" xr:uid="{889C3BDC-78B4-6648-9AA3-AA7E82A3B939}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="N15" xr:uid="{C8359500-4E3F-5444-8C3A-7A9C12536A5E}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Click and enter a value from the list" sqref="N16:N150 O15:O150" xr:uid="{9CAFE2A0-7485-1B45-821B-616F3E6537DA}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Click and enter a value from the list" sqref="I15:I150" xr:uid="{EB58CC99-0E9B-A94A-9E5D-26F4AF211845}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Click and enter a value from the list" sqref="N16:N150 O15:O150 I15:I150" xr:uid="{9CAFE2A0-7485-1B45-821B-616F3E6537DA}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" display="detailed information about variant types and information required can be found here " xr:uid="{F6DA5A5D-A5B6-E94D-A379-D37068779481}"/>
@@ -47775,17 +47767,17 @@
           </x14:formula1>
           <xm:sqref>H15:H151 I151</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BB544530-0A53-3B44-8698-63431308BE25}">
-          <x14:formula1>
-            <xm:f>Lookups!$I$2:$I$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>W15:W152</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FED8FDE5-1EAF-2C42-96F0-6CE276B9A504}">
           <x14:formula1>
             <xm:f>Lookups!$G$2:$G$33</xm:f>
           </x14:formula1>
           <xm:sqref>Z15:Z150</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BB544530-0A53-3B44-8698-63431308BE25}">
+          <x14:formula1>
+            <xm:f>Lookups!$I$2:$I$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>W17:W152 W15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
ZFIN-6928 updated workbook to open at A1
</commit_message>
<xml_diff>
--- a/home/zf_info/zebraShareSubmission.xlsx
+++ b/home/zf_info/zebraShareSubmission.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/administrator/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pritamani/wfh16/releases/1120/ZFIN_WWW/home/zf_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C177438D-F0ED-3D4C-98F7-4280140579FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{93A2E3AC-096C-544B-8AF6-21E6F8B955AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="460" windowWidth="31720" windowHeight="17340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5320" yWindow="460" windowWidth="45880" windowHeight="26540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -2912,6 +2912,50 @@
     <xf numFmtId="0" fontId="26" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2920,12 +2964,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2944,19 +2982,10 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2975,35 +3004,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -4424,9 +4424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:NB1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD7" sqref="AD7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4481,14 +4479,14 @@
       <c r="I1" s="73"/>
       <c r="J1" s="75"/>
       <c r="K1" s="75"/>
-      <c r="L1" s="135" t="s">
+      <c r="L1" s="131" t="s">
         <v>178</v>
       </c>
-      <c r="M1" s="136"/>
-      <c r="N1" s="136"/>
-      <c r="O1" s="136"/>
-      <c r="P1" s="136"/>
-      <c r="Q1" s="136"/>
+      <c r="M1" s="132"/>
+      <c r="N1" s="132"/>
+      <c r="O1" s="132"/>
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
       <c r="U1" s="77"/>
       <c r="AN1" s="78"/>
       <c r="AO1" s="78"/>
@@ -4879,14 +4877,14 @@
       <c r="U4" s="77"/>
     </row>
     <row r="5" spans="1:366" s="84" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="135" t="s">
+      <c r="A5" s="131" t="s">
         <v>223</v>
       </c>
-      <c r="B5" s="136"/>
-      <c r="C5" s="136"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
+      <c r="B5" s="132"/>
+      <c r="C5" s="132"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="132"/>
       <c r="G5" s="83"/>
       <c r="H5" s="86"/>
       <c r="J5" s="86"/>
@@ -5233,11 +5231,11 @@
       <c r="C6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="131" t="s">
+      <c r="D6" s="145" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="132"/>
-      <c r="F6" s="132"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="146"/>
       <c r="G6" s="20" t="s">
         <v>7</v>
       </c>
@@ -5319,11 +5317,11 @@
       <c r="AG6" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="AH6" s="133" t="s">
+      <c r="AH6" s="147" t="s">
         <v>126</v>
       </c>
-      <c r="AI6" s="134"/>
-      <c r="AJ6" s="134"/>
+      <c r="AI6" s="148"/>
+      <c r="AJ6" s="148"/>
       <c r="AK6" s="15" t="s">
         <v>87</v>
       </c>
@@ -7993,13 +7991,13 @@
       <c r="NB12"/>
     </row>
     <row r="13" spans="1:366" s="19" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="139" t="s">
+      <c r="A13" s="151" t="s">
         <v>229</v>
       </c>
-      <c r="B13" s="141" t="s">
+      <c r="B13" s="153" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="141" t="s">
+      <c r="C13" s="153" t="s">
         <v>103</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -8014,16 +8012,16 @@
       <c r="G13" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="137" t="s">
+      <c r="H13" s="149" t="s">
         <v>59</v>
       </c>
       <c r="I13" s="100" t="s">
         <v>157</v>
       </c>
-      <c r="J13" s="141" t="s">
+      <c r="J13" s="153" t="s">
         <v>148</v>
       </c>
-      <c r="K13" s="141">
+      <c r="K13" s="153">
         <v>10</v>
       </c>
       <c r="L13" s="95" t="s">
@@ -8038,72 +8036,72 @@
       <c r="O13" s="97" t="s">
         <v>196</v>
       </c>
-      <c r="P13" s="143" t="s">
+      <c r="P13" s="135" t="s">
         <v>143</v>
       </c>
-      <c r="Q13" s="145" t="s">
+      <c r="Q13" s="155" t="s">
         <v>206</v>
       </c>
-      <c r="R13" s="147" t="s">
+      <c r="R13" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="S13" s="156" t="s">
+      <c r="S13" s="137" t="s">
         <v>129</v>
       </c>
-      <c r="T13" s="147" t="s">
+      <c r="T13" s="139" t="s">
         <v>28</v>
       </c>
-      <c r="U13" s="159" t="s">
+      <c r="U13" s="141" t="s">
         <v>28</v>
       </c>
-      <c r="V13" s="161" t="s">
+      <c r="V13" s="143" t="s">
         <v>28</v>
       </c>
       <c r="W13" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="X13" s="141" t="s">
+      <c r="X13" s="153" t="s">
         <v>107</v>
       </c>
-      <c r="Y13" s="150" t="s">
+      <c r="Y13" s="159" t="s">
         <v>29</v>
       </c>
-      <c r="Z13" s="147" t="s">
+      <c r="Z13" s="139" t="s">
         <v>30</v>
       </c>
-      <c r="AA13" s="152" t="s">
+      <c r="AA13" s="161" t="s">
         <v>130</v>
       </c>
       <c r="AB13" s="107" t="s">
         <v>163</v>
       </c>
       <c r="AC13" s="107"/>
-      <c r="AD13" s="143" t="s">
+      <c r="AD13" s="135" t="s">
         <v>155</v>
       </c>
       <c r="AE13" s="124"/>
-      <c r="AF13" s="143" t="s">
+      <c r="AF13" s="135" t="s">
         <v>155</v>
       </c>
-      <c r="AG13" s="143" t="s">
+      <c r="AG13" s="135" t="s">
         <v>155</v>
       </c>
-      <c r="AH13" s="143" t="s">
+      <c r="AH13" s="135" t="s">
         <v>155</v>
       </c>
-      <c r="AI13" s="143" t="s">
+      <c r="AI13" s="135" t="s">
         <v>155</v>
       </c>
-      <c r="AJ13" s="143" t="s">
+      <c r="AJ13" s="135" t="s">
         <v>155</v>
       </c>
-      <c r="AK13" s="154" t="s">
+      <c r="AK13" s="133" t="s">
         <v>164</v>
       </c>
-      <c r="AL13" s="154" t="s">
+      <c r="AL13" s="133" t="s">
         <v>165</v>
       </c>
-      <c r="AM13" s="143" t="s">
+      <c r="AM13" s="135" t="s">
         <v>155</v>
       </c>
       <c r="AN13"/>
@@ -8435,9 +8433,9 @@
       <c r="NB13"/>
     </row>
     <row r="14" spans="1:366" s="64" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="140"/>
-      <c r="B14" s="142"/>
-      <c r="C14" s="142"/>
+      <c r="A14" s="152"/>
+      <c r="B14" s="154"/>
+      <c r="C14" s="154"/>
       <c r="D14" s="102" t="s">
         <v>40</v>
       </c>
@@ -8450,12 +8448,12 @@
       <c r="G14" s="101" t="s">
         <v>106</v>
       </c>
-      <c r="H14" s="138"/>
+      <c r="H14" s="150"/>
       <c r="I14" s="99" t="s">
         <v>154</v>
       </c>
-      <c r="J14" s="142"/>
-      <c r="K14" s="142"/>
+      <c r="J14" s="154"/>
+      <c r="K14" s="154"/>
       <c r="L14" s="98" t="s">
         <v>199</v>
       </c>
@@ -8468,30 +8466,30 @@
       <c r="O14" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="P14" s="144"/>
-      <c r="Q14" s="146"/>
-      <c r="R14" s="148"/>
-      <c r="S14" s="157"/>
-      <c r="T14" s="158"/>
-      <c r="U14" s="160"/>
-      <c r="V14" s="162"/>
+      <c r="P14" s="136"/>
+      <c r="Q14" s="156"/>
+      <c r="R14" s="157"/>
+      <c r="S14" s="138"/>
+      <c r="T14" s="140"/>
+      <c r="U14" s="142"/>
+      <c r="V14" s="144"/>
       <c r="W14" s="128"/>
-      <c r="X14" s="149"/>
-      <c r="Y14" s="151"/>
-      <c r="Z14" s="148"/>
-      <c r="AA14" s="153"/>
+      <c r="X14" s="158"/>
+      <c r="Y14" s="160"/>
+      <c r="Z14" s="157"/>
+      <c r="AA14" s="162"/>
       <c r="AB14" s="108"/>
       <c r="AC14" s="108"/>
-      <c r="AD14" s="144"/>
+      <c r="AD14" s="136"/>
       <c r="AE14" s="125"/>
-      <c r="AF14" s="144"/>
-      <c r="AG14" s="144"/>
-      <c r="AH14" s="144"/>
-      <c r="AI14" s="144"/>
-      <c r="AJ14" s="144"/>
-      <c r="AK14" s="155"/>
-      <c r="AL14" s="155"/>
-      <c r="AM14" s="144"/>
+      <c r="AF14" s="136"/>
+      <c r="AG14" s="136"/>
+      <c r="AH14" s="136"/>
+      <c r="AI14" s="136"/>
+      <c r="AJ14" s="136"/>
+      <c r="AK14" s="134"/>
+      <c r="AL14" s="134"/>
+      <c r="AM14" s="136"/>
       <c r="AN14" s="55"/>
       <c r="AO14" s="55"/>
       <c r="AP14" s="55"/>
@@ -49699,20 +49697,6 @@
   <sheetProtection selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="30">
-    <mergeCell ref="L1:Q1"/>
-    <mergeCell ref="AK13:AK14"/>
-    <mergeCell ref="AL13:AL14"/>
-    <mergeCell ref="AM13:AM14"/>
-    <mergeCell ref="AD13:AD14"/>
-    <mergeCell ref="AF13:AF14"/>
-    <mergeCell ref="AG13:AG14"/>
-    <mergeCell ref="AH13:AH14"/>
-    <mergeCell ref="AI13:AI14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="AJ13:AJ14"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="AH6:AJ6"/>
     <mergeCell ref="A5:F5"/>
@@ -49729,6 +49713,20 @@
     <mergeCell ref="Y13:Y14"/>
     <mergeCell ref="Z13:Z14"/>
     <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="AK13:AK14"/>
+    <mergeCell ref="AL13:AL14"/>
+    <mergeCell ref="AM13:AM14"/>
+    <mergeCell ref="AD13:AD14"/>
+    <mergeCell ref="AF13:AF14"/>
+    <mergeCell ref="AG13:AG14"/>
+    <mergeCell ref="AH13:AH14"/>
+    <mergeCell ref="AI13:AI14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="AJ13:AJ14"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="4">

</xml_diff>